<commit_message>
-> BOM: correction C12;C14 mouser reference
</commit_message>
<xml_diff>
--- a/Hardware/D0018N4102-002 BOM 16 channels v10.xlsx
+++ b/Hardware/D0018N4102-002 BOM 16 channels v10.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="100">
   <si>
     <t xml:space="preserve"> Footprint</t>
   </si>
@@ -163,15 +163,6 @@
     <t>2,2kohm/1%</t>
   </si>
   <si>
-    <t>C0805C475K8PAC7210</t>
-  </si>
-  <si>
-    <t>4,7uF/10V/X5R</t>
-  </si>
-  <si>
-    <t>80-C0805C475K8PACLR</t>
-  </si>
-  <si>
     <t>R4;R17;R16;R14;R25;R24;R22;R15;R23;R21;R20;R18;R29;R28;R26;R19;R27</t>
   </si>
   <si>
@@ -308,6 +299,21 @@
   </si>
   <si>
     <t>DNP</t>
+  </si>
+  <si>
+    <t>4,7uF/25V/X7R</t>
+  </si>
+  <si>
+    <t>VJ126Y475KXXTW1BC</t>
+  </si>
+  <si>
+    <t>Vishay</t>
+  </si>
+  <si>
+    <t>77-VJ126Y475KXXTW1BC</t>
+  </si>
+  <si>
+    <t>SMD1206</t>
   </si>
 </sst>
 </file>
@@ -1164,7 +1170,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C10" sqref="C10:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1210,7 +1216,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -1233,19 +1239,19 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" t="s">
         <v>93</v>
-      </c>
-      <c r="D3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G3" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1374,13 +1380,13 @@
         <v>48</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G9" t="s">
         <v>36</v>
@@ -1394,39 +1400,39 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>96</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>51</v>
+        <v>98</v>
       </c>
       <c r="G10" t="s">
-        <v>36</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B11">
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G11" t="s">
         <v>36</v>
@@ -1434,22 +1440,22 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B12">
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="G12" t="s">
         <v>36</v>
@@ -1463,10 +1469,10 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D13" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G13" t="s">
         <v>36</v>
@@ -1474,22 +1480,22 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G14" t="s">
         <v>36</v>
@@ -1497,22 +1503,22 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="D15" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" t="s">
-        <v>70</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="G15" t="s">
         <v>36</v>
@@ -1526,19 +1532,19 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D16" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E16" t="s">
         <v>25</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1549,59 +1555,59 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D17" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D18" t="s">
         <v>9</v>
       </c>
       <c r="E18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G18" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B19">
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D19" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E19" t="s">
         <v>25</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G19" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1612,19 +1618,19 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D20" t="s">
         <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G20" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1635,17 +1641,17 @@
     <hyperlink ref="F6" r:id="rId4" tooltip="Clique para visualizar informações adicionais sobre este produto" display="https://pt.mouser.com/ProductDetail/KEMET/C0805C104M5RAC7210?qs=sGAEpiMZZMs0AnBnWHyRQFCCI5cSbRT%2fI0VuIi6eznI%3d"/>
     <hyperlink ref="F7" r:id="rId5" tooltip="Clique para visualizar informações adicionais sobre este produto" display="https://pt.mouser.com/ProductDetail/IQD/LFXTAL066898Reel?qs=sGAEpiMZZMsBj6bBr9Q9aR%2fuGiDjvlISxfF6EyUKh0QY%252bn1mC20qZQ%3d%3d"/>
     <hyperlink ref="F8" r:id="rId6" tooltip="Clique para visualizar informações adicionais sobre este produto" display="https://pt.mouser.com/ProductDetail/KEMET/C0805C120J5GAC7210?qs=sGAEpiMZZMs0AnBnWHyRQOf5HOpVaXbhAZEuEA3l7uw%3d"/>
-    <hyperlink ref="F10" r:id="rId7" tooltip="Clique para visualizar informações adicionais sobre este produto" display="https://pt.mouser.com/ProductDetail/KEMET/C0805C475K8PAC7210?qs=sGAEpiMZZMs0AnBnWHyRQHefeAIkSpb%2fgNRE2hi4Qhw%3d"/>
-    <hyperlink ref="F11" r:id="rId8" tooltip="Clique para visualizar informações adicionais sobre este produto" display="https://pt.mouser.com/ProductDetail/Yageo/RT0805FRE0710KL?qs=sGAEpiMZZMu61qfTUdNhGxEjuuBLd0B41oWml1pU2QE%3d"/>
-    <hyperlink ref="F12" r:id="rId9" tooltip="Clique para visualizar informações adicionais sobre este produto" display="https://pt.mouser.com/ProductDetail/Yageo/RT0805FRE07100KL?qs=sGAEpiMZZMu61qfTUdNhGxEjuuBLd0B4mFnwhs6X5Kw%3d"/>
-    <hyperlink ref="F9" r:id="rId10" tooltip="Clique para visualizar informações adicionais sobre este produto" display="https://pt.mouser.com/ProductDetail/Yageo/RT0805DRD072K2L?qs=sGAEpiMZZMu61qfTUdNhGxEjuuBLd0B4GZ1bCnPt7TI%3d"/>
-    <hyperlink ref="F14" r:id="rId11" tooltip="Clique para visualizar informações adicionais sobre este produto" display="https://pt.mouser.com/ProductDetail/Yageo/RC0805FR-070RL?qs=sGAEpiMZZMu61qfTUdNhG6gKAQVNBKOonL%252bE%2fLYSU34%3d"/>
-    <hyperlink ref="F15" r:id="rId12" tooltip="Clique para visualizar informações adicionais sobre este produto" display="https://pt.mouser.com/ProductDetail/Kingbright/APT2012SGC?qs=sGAEpiMZZMvyj6n1w4pZD5QO%2fJ%252bHmnjZlXC14XYqTf8%3d"/>
-    <hyperlink ref="F16" r:id="rId13" tooltip="Clique para visualizar informações adicionais sobre este produto" display="https://pt.mouser.com/ProductDetail/STMicroelectronics/M24128-DFMN6TP?qs=sGAEpiMZZMuVhdAcoizlRSnLhVfhSoFzqdBPoNcIiYg%3d"/>
-    <hyperlink ref="F18" r:id="rId14" tooltip="Clique para visualizar informações adicionais sobre este produto" display="https://pt.mouser.com/ProductDetail/Texas-Instruments/SN74LVC245APWR?qs=sGAEpiMZZMs9F6aVvY09bnFMVNxjj%2fgIjJoUJoCdNnE%3d"/>
-    <hyperlink ref="F19" r:id="rId15" tooltip="Clique para visualizar informações adicionais sobre este produto" display="https://pt.mouser.com/ProductDetail/STMicroelectronics/USBLC6-4SC6?qs=sGAEpiMZZMvxHShE6Whpu7uDi%252bhiPVjaQjZOzaiLtNs%3d"/>
-    <hyperlink ref="F20" r:id="rId16" tooltip="Clique para visualizar informações adicionais sobre este produto" display="https://pt.mouser.com/ProductDetail/TE-Connectivity-AMP/5-146130-8?qs=sGAEpiMZZMs%252bGHln7q6pm%2f6BrHToExQ46GhDhc3%252bFaE%3d"/>
-    <hyperlink ref="F3" r:id="rId17" tooltip="Clique para visualizar informações adicionais sobre este produto" display="https://pt.mouser.com/ProductDetail/CUI/UJ2-MBH-1-SMT-TR?qs=sGAEpiMZZMulM8LPOQ%252byk%252br6FietFiXBYOK8b9%2fsuNIy0pbKqeLWLA%3d%3d"/>
+    <hyperlink ref="F11" r:id="rId7" tooltip="Clique para visualizar informações adicionais sobre este produto" display="https://pt.mouser.com/ProductDetail/Yageo/RT0805FRE0710KL?qs=sGAEpiMZZMu61qfTUdNhGxEjuuBLd0B41oWml1pU2QE%3d"/>
+    <hyperlink ref="F12" r:id="rId8" tooltip="Clique para visualizar informações adicionais sobre este produto" display="https://pt.mouser.com/ProductDetail/Yageo/RT0805FRE07100KL?qs=sGAEpiMZZMu61qfTUdNhGxEjuuBLd0B4mFnwhs6X5Kw%3d"/>
+    <hyperlink ref="F9" r:id="rId9" tooltip="Clique para visualizar informações adicionais sobre este produto" display="https://pt.mouser.com/ProductDetail/Yageo/RT0805DRD072K2L?qs=sGAEpiMZZMu61qfTUdNhGxEjuuBLd0B4GZ1bCnPt7TI%3d"/>
+    <hyperlink ref="F14" r:id="rId10" tooltip="Clique para visualizar informações adicionais sobre este produto" display="https://pt.mouser.com/ProductDetail/Yageo/RC0805FR-070RL?qs=sGAEpiMZZMu61qfTUdNhG6gKAQVNBKOonL%252bE%2fLYSU34%3d"/>
+    <hyperlink ref="F15" r:id="rId11" tooltip="Clique para visualizar informações adicionais sobre este produto" display="https://pt.mouser.com/ProductDetail/Kingbright/APT2012SGC?qs=sGAEpiMZZMvyj6n1w4pZD5QO%2fJ%252bHmnjZlXC14XYqTf8%3d"/>
+    <hyperlink ref="F16" r:id="rId12" tooltip="Clique para visualizar informações adicionais sobre este produto" display="https://pt.mouser.com/ProductDetail/STMicroelectronics/M24128-DFMN6TP?qs=sGAEpiMZZMuVhdAcoizlRSnLhVfhSoFzqdBPoNcIiYg%3d"/>
+    <hyperlink ref="F18" r:id="rId13" tooltip="Clique para visualizar informações adicionais sobre este produto" display="https://pt.mouser.com/ProductDetail/Texas-Instruments/SN74LVC245APWR?qs=sGAEpiMZZMs9F6aVvY09bnFMVNxjj%2fgIjJoUJoCdNnE%3d"/>
+    <hyperlink ref="F19" r:id="rId14" tooltip="Clique para visualizar informações adicionais sobre este produto" display="https://pt.mouser.com/ProductDetail/STMicroelectronics/USBLC6-4SC6?qs=sGAEpiMZZMvxHShE6Whpu7uDi%252bhiPVjaQjZOzaiLtNs%3d"/>
+    <hyperlink ref="F20" r:id="rId15" tooltip="Clique para visualizar informações adicionais sobre este produto" display="https://pt.mouser.com/ProductDetail/TE-Connectivity-AMP/5-146130-8?qs=sGAEpiMZZMs%252bGHln7q6pm%2f6BrHToExQ46GhDhc3%252bFaE%3d"/>
+    <hyperlink ref="F3" r:id="rId16" tooltip="Clique para visualizar informações adicionais sobre este produto" display="https://pt.mouser.com/ProductDetail/CUI/UJ2-MBH-1-SMT-TR?qs=sGAEpiMZZMulM8LPOQ%252byk%252br6FietFiXBYOK8b9%2fsuNIy0pbKqeLWLA%3d%3d"/>
+    <hyperlink ref="F10" r:id="rId17" tooltip="Clique para visualizar informações adicionais sobre este produto" display="https://pt.mouser.com/ProductDetail/Vishay-Vitramon/VJ1206Y475KXXTW1BC?qs=sGAEpiMZZMs0AnBnWHyRQN7%2fAA2D2lPPu%252b7jaAAvyUeBMMU%2fzrdczQ%3d%3d"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId18"/>

</xml_diff>